<commit_message>
correction 1.5 avec cours de M
</commit_message>
<xml_diff>
--- a/prepa_certif_updated_scrum_questions_faites.xlsx
+++ b/prepa_certif_updated_scrum_questions_faites.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\formation_BA\Nouveau dossier\prepa_certif\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15819C46-58CA-4F57-A59A-715728E819C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EA0A30C-EB44-4DEE-A19D-D8F047351397}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,24 +30,9 @@
     <t>Burndown chart</t>
   </si>
   <si>
-    <t>Sprint Review</t>
-  </si>
-  <si>
-    <t>Sprint rétrospective</t>
-  </si>
-  <si>
-    <t>Daily Scrum</t>
-  </si>
-  <si>
     <t>Product backlog</t>
   </si>
   <si>
-    <t>DONE</t>
-  </si>
-  <si>
-    <t>Backlog Refinement</t>
-  </si>
-  <si>
     <t>scrum team</t>
   </si>
   <si>
@@ -55,9 +40,6 @@
   </si>
   <si>
     <t>Sprint backlog</t>
-  </si>
-  <si>
-    <t>Sprint planning</t>
   </si>
   <si>
     <t xml:space="preserve">Sprint </t>
@@ -127,170 +109,6 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> est pour le PO.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">3 heures max, cérémonie scrum en fermeture du sprint qui se réalise juste après la sprint Review. C'est pour les developers (ou pour la scrum team, donc le PO y participe et peut adapter le "done". 
-( pour les processus) Sert à </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>améliorer</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> pour les prochains sprints, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>identifier</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> ce qui a été bien et qui a du potentiel d'amélioration, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>analyser</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> ce qui s'est passé &gt;&gt; &gt;&gt;&gt; people, relationships, process, and tool.
-if </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>improvement</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> possible, include at least 1 high priority process for the next.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">8h max (4h/2semaines, 8h/1mois), responsable: scrum team, pas la place des key stakeholders mais ils peuvent y assister.
-Participants : la scrum team (scrum master, product owner, developers). Others possible to provide </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>technical advice</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">.
-Comment le travail sera fait pour le prochain increment ? (work needed to deliver)
-Qu'est-ce qui sera livré? (delivered in the Increment resulting).
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">input </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: last sprint, product backlog, past performance, last increment.
-L'important est la plannification </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>des premiers jours</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
     </r>
   </si>
   <si>
@@ -395,35 +213,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Plan of work for next 24h, inspecting work since the last, forecasting upcoming sprint work.
-Dev team, 15 minutes peu importe la taille de l'équipe, tous les jours, le matin ou l'après-midi.
-PAS DE FORMAT DEFINI : </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>questions ou discussion, tout est possible</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, le scrum master ne la "conduit" pas.
-3 questions du scrum master : je vois les obstacles qui empêchent d'aller au but, j'ai vu hier ce qui peut aider les developers, je peux les aider aujourd'hui à atteindre ce but. --NO CANCELLATION ALLOWED--.</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">Developers (responsable du suivi du travail restant), la définition de "done" </t>
     </r>
     <r>
@@ -619,222 +408,10 @@
     </r>
   </si>
   <si>
-    <t>ils mélangent les versions (ancienne-nouvelle) dans les questions de la certif. Si dans la question, dev team : ancienne, si developers : nouvelle.</t>
-  </si>
-  <si>
-    <t>au 01/03/21, certifs obtenues avec Mourad durant sa session de décembre : 8sm 6po</t>
-  </si>
-  <si>
     <t>the Stakeholders</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Pour toute question où il y a la notion d'obligation, la réponse sera </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>FALSE</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
     <t>proxy PO : son adjoint</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Responsable : PO uniquement.
-Les developers peuvent faire des changements </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>avec l'accord du PO (attention au sens de la question)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Les developers sont responsable des </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">estimations.      </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Any technique should be used for </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>representing</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> product backlog items.
-developers </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>should</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> use the same product backlog.    </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Ready</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> : well refined, at the top, can be done in 1 sprint.
-&gt; dynamic, never complete, existe tant que le produit existe.
-C'est </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>la seule source</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> pour tout changement du produit.     </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Optionnel</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> : tests prouvant le "done" et les dépendances.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Management : </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">PO responsable.
-</t>
-    </r>
   </si>
   <si>
     <r>
@@ -1138,145 +715,6 @@
   </si>
   <si>
     <t>Le mot scrum est apparu en 1995, l'agilité en 2001, le scrum guide en 2010.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Le PO, developers. BEFORE : "consume not more than 10% of the capacity of the developers"    NOW : à l'appréciation.
-Not for the current sprint in progress.
-Ongoing process, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>act of adding detail</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Cancellation</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> : PO only (OR </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>if sprint goal obsolete ( ou inatteignable)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">).
-Longueur maximale : 1 mois sinon, pas de norme selon de scrum guide MAIS on établit sa </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>longueur</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> en fonction : de la possibilité d'être en réunion avec les stakeholders et des "done" pouvant être faits + fréquemment.
-La qualité ne doit pas baisser, l'objectif ne doit pas être mis en danger, scope may be clarified and re-negociated.
-Le sprint est le SEUL moment dans lequel </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>on n'inspecte pas et on n'adapte pas</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">At the end </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>of the sprint : the delivery is working, functional, DONE.</t>
-    </r>
   </si>
   <si>
     <t>4 heures max, but : présenter le produit (travail réalisé) durant le sprint en cours OU "a revisited product backlog". 
@@ -1386,8 +824,15 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">C'est un servant, helping developers to create value, removing impediments, coaching the developers.
+    <t>ils mélangent les versions (ancienne/nouvelle) dans les questions de la certif. Si dans la question, il y a "dev team" : ancienne, 
+si "developers" : nouvelle.</t>
+  </si>
+  <si>
+    <t>Definition of DONE</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">C'est un servant leader sans pouvoir, helping developers to create value, removing impediments, coaching the developers.
 </t>
     </r>
     <r>
@@ -1453,8 +898,602 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> and teaching scrum events, techniques for product backlog management, empirical env.
+      <t xml:space="preserve"> and teaching scrum events, </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>techniques for product backlog management</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, empirical env.
 Si le PO a des soucis avec les user stories, il peut les rédiger.</t>
+    </r>
+  </si>
+  <si>
+    <t>Sprint Review
+(événement scrum)</t>
+  </si>
+  <si>
+    <t>Sprint rétrospective
+(événement scrum)</t>
+  </si>
+  <si>
+    <t>Sprint planning
+(événement scrum)</t>
+  </si>
+  <si>
+    <t>Daily Scrum
+(événement scrum)</t>
+  </si>
+  <si>
+    <t>1 mois : 20 jours de travail.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Cancellation</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : PO only (OR </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>if sprint goal obsolete ( ou inatteignable)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">). Le sprint zero n'existe pas.
+Longueur maximale : 1 mois sinon, pas de norme selon de scrum guide MAIS on établit sa </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>longueur</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> en fonction : de la possibilité d'être en réunion avec les stakeholders et des "done" pouvant être faits + fréquemment.
+La qualité ne doit pas baisser, l'objectif ne doit pas être mis en danger, scope may be clarified and re-negociated.
+Le sprint est le SEUL moment dans lequel </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>on n'inspecte pas et on n'adapte pas</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">.
+Durant le sprint &gt; choix des besoins livrables le mois, spec f, dev, test, livraison.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">At the end </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>of the sprint : the delivery is working, functional, DONE.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Plan of work for next 24h, inspecting work since the last, forecasting upcoming sprint work.
+Dev team, 15 minutes peu importe la taille de l'équipe, debout ou pas, tous les jours, le matin ou l'après-midi.
+BEFORE : 3 questions &gt; hier, aujourd'hui, blocages. NOW : </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">questions ou discussion, tout est possible.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Le scrum master ne la "conduit" pas.
+3 questions du scrum master : je vois les obstacles qui empêchent d'aller au but, j'ai vu hier ce qui peut aider les developers, je peux les aider aujourd'hui à atteindre ce but. --NO CANCELLATION ALLOWED--.</t>
+    </r>
+  </si>
+  <si>
+    <t>Backlog Refinement 
+ou Grooming
+(non événement)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Le PO, developers. BEFORE : "consume not more than 10% of the capacity of the developers"    NOW : à l'appréciation.
+Not for the current sprint in progress, on prépare le sprint suivant à la mi-sprint, durée à la convenance.
+Ongoing process, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>act of adding detail</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Responsable : PO uniquement.
+Les developers peuvent faire des changements </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>avec l'accord du PO (attention au sens de la question)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Les developers sont responsable des </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">estimations.      </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Any technique should be used for </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>representing</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> product backlog items. Ce qui n'est pas fini n'est pas reporté au prochain sprint, c'est mis dans le product backlog.
+developers </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>should</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> use the same product backlog.    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ready</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : well refined, at the top, can be done in 1 sprint.
+&gt; dynamic, never complete, existe tant que le produit existe.
+C'est </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>la seule source</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> pour tout changement du produit.     </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Optionnel</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : tests prouvant le "done" et les dépendances.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Management : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">PO responsable.
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">3 heures max, cérémonie scrum en fermeture du sprint qui se réalise juste après la sprint Review. C'est pour la scrum team, donc le PO y participe et peut adapter le "done". 
+( pour les processus) Sert à </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>améliorer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> pour les prochains sprints, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>identifier</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ce qui a été bien et qui a du potentiel d'amélioration, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>analyser</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ce qui s'est passé &gt;&gt; &gt;&gt;&gt; people, relationships, process, and tool.
+if </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>improvement</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> possible, include at least 1 high priority process for the next.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Pour toute question où il y a la notion d'obligation, la réponse sera </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>FALSE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">8h max (4h/2semaines, 8h/1mois), responsable: scrum team, pas la place des stakeholders mais ils peuvent y assister.
+Participants : la scrum team (scrum master, product owner, developers). Others possible to provide </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>technical advice</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">.
+Comment le travail sera fait pour le prochain increment ? (work needed to deliver)
+Qu'est-ce qui sera livré? (delivered in the Increment resulting).
+Le BA rédige les user stories.
+les questions sur le choix des user stories : why, what, how. 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">input </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: last sprint, product backlog, past performance, last increment.
+L'important est la plannification </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>des premiers jours</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Les developers se défendent avec la vélocité.</t>
     </r>
   </si>
 </sst>
@@ -1462,7 +1501,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1550,13 +1589,52 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0066"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1571,7 +1649,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1591,12 +1669,29 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF0066"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1871,217 +1966,219 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="18" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23.109375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="98.44140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="32.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="76.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="24.77734375" style="1" customWidth="1"/>
     <col min="4" max="4" width="29.6640625" style="1" customWidth="1"/>
     <col min="5" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="23.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="23.4" x14ac:dyDescent="0.3">
       <c r="C1" s="6" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="136.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="161.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>30</v>
-      </c>
     </row>
-    <row r="3" spans="1:4" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="4"/>
     </row>
-    <row r="4" spans="1:4" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="60.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="12.45" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:3" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="12.45" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:3" ht="79.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="12.45" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:3" ht="159" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C10" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="12.6" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:3" ht="174" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="9"/>
+    </row>
+    <row r="14" spans="1:3" ht="165.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="12.45" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:3" ht="84.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
         <v>32</v>
       </c>
+      <c r="B16" s="2" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" ht="12.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:4" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="2" t="s">
+    <row r="17" spans="1:3" ht="12.45" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="18" spans="1:3" ht="102" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="12.45" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="12.45" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:3" ht="190.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="12.45" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="1:3" ht="147" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>25</v>
-      </c>
     </row>
-    <row r="7" spans="1:4" ht="12.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:4" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
+    <row r="25" spans="1:3" ht="12.45" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="1:3" ht="135" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="12.45" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="1:3" ht="160.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="12.45" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:3" ht="184.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>38</v>
+      <c r="B30" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="12.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:4" ht="98.55" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="12.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="12.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:4" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="12.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:4" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B16" s="2" t="s">
+    <row r="31" spans="1:3" ht="12.45" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="1:3" ht="161.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="12.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="18" spans="1:2" ht="105" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="12.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="20" spans="1:2" ht="81" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="12.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="12.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="24" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="12.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="26" spans="1:2" ht="109.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="12.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="28" spans="1:2" ht="144" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="12.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="1:2" ht="103.2" x14ac:dyDescent="0.3">
-      <c r="A30" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="12.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="32" spans="1:2" ht="144" x14ac:dyDescent="0.3">
-      <c r="A32" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="12.6" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="34" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" ht="144" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="12.6" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="36" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="38" spans="1:2" ht="91.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
correction 2 avec cours de M
</commit_message>
<xml_diff>
--- a/prepa_certif_updated_scrum_questions_faites.xlsx
+++ b/prepa_certif_updated_scrum_questions_faites.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\formation_BA\Nouveau dossier\prepa_certif\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EA0A30C-EB44-4DEE-A19D-D8F047351397}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64D3C9D8-F93B-4BAD-8987-051ED0F6A525}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
   <si>
     <t>Burndown chart</t>
   </si>
@@ -40,9 +40,6 @@
   </si>
   <si>
     <t>Sprint backlog</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sprint </t>
   </si>
   <si>
     <t xml:space="preserve">Scrum </t>
@@ -313,9 +310,6 @@
     <t>DIVERS</t>
   </si>
   <si>
-    <t>association avec PMI-ACP : être moins prescriptif mais plus descriptif d'où les changements.</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -717,8 +711,478 @@
     <t>Le mot scrum est apparu en 1995, l'agilité en 2001, le scrum guide en 2010.</t>
   </si>
   <si>
-    <t>4 heures max, but : présenter le produit (travail réalisé) durant le sprint en cours OU "a revisited product backlog". 
-C'est pour les stakeholders, scrum master, developers, PO.    It's not JUST a demo et possible de ne rien livrer.</t>
+    <t>ils mélangent les versions (ancienne/nouvelle) dans les questions de la certif. Si dans la question, il y a "dev team" : ancienne, 
+si "developers" : nouvelle.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">C'est un servant leader sans pouvoir, helping developers to create value, removing impediments, coaching the developers.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Is responsible for conducting the Daily Scrum</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. NOW : Il est </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>responsable</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> de la réussite de la scrum team.
+Leading &amp; coaching org, working with other scrum masters, planning scrum implementations.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Facilitating</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and teaching scrum events, </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>techniques for product backlog management</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, empirical env.
+Si le PO a des soucis avec les user stories, il peut les rédiger.</t>
+    </r>
+  </si>
+  <si>
+    <t>Sprint Review
+(événement scrum)</t>
+  </si>
+  <si>
+    <t>Sprint rétrospective
+(événement scrum)</t>
+  </si>
+  <si>
+    <t>Sprint planning
+(événement scrum)</t>
+  </si>
+  <si>
+    <t>Daily Scrum
+(événement scrum)</t>
+  </si>
+  <si>
+    <t>1 mois : 20 jours de travail.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Cancellation</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : PO only (OR </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>if sprint goal obsolete ( ou inatteignable)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">). Le sprint zero n'existe pas.
+Longueur maximale : 1 mois sinon, pas de norme selon de scrum guide MAIS on établit sa </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>longueur</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> en fonction : de la possibilité d'être en réunion avec les stakeholders et des "done" pouvant être faits + fréquemment.
+La qualité ne doit pas baisser, l'objectif ne doit pas être mis en danger, scope may be clarified and re-negociated.
+Le sprint est le SEUL moment dans lequel </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>on n'inspecte pas et on n'adapte pas</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">.
+Durant le sprint &gt; choix des besoins livrables le mois, spec f, dev, test, livraison.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">At the end </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>of the sprint : the delivery is working, functional, DONE.</t>
+    </r>
+  </si>
+  <si>
+    <t>Backlog Refinement 
+ou Grooming
+(non événement)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Le PO, developers. BEFORE : "consume not more than 10% of the capacity of the developers"    NOW : à l'appréciation.
+Not for the current sprint in progress, on prépare le sprint suivant à la mi-sprint, durée à la convenance.
+Ongoing process, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>act of adding detail</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Responsable : PO uniquement.
+Les developers peuvent faire des changements </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>avec l'accord du PO (attention au sens de la question)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Les developers sont responsable des </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">estimations.      </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Any technique should be used for </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>representing</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> product backlog items. Ce qui n'est pas fini n'est pas reporté au prochain sprint, c'est mis dans le product backlog.
+developers </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>should</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> use the same product backlog.    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ready</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : well refined, at the top, can be done in 1 sprint.
+&gt; dynamic, never complete, existe tant que le produit existe.
+C'est </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>la seule source</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> pour tout changement du produit.     </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Optionnel</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : tests prouvant le "done" et les dépendances.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Management : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">PO responsable.
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Pour toute question où il y a la notion d'obligation, la réponse sera </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">FALSE </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(le but est de réduire les obligations).</t>
+    </r>
+  </si>
+  <si>
+    <t>Sprint 
+(événement scrum)</t>
+  </si>
+  <si>
+    <t>association avec PMI-ACP : être moins prescriptif mais plus descriptif d'où les changements dans le scrum guide.</t>
   </si>
   <si>
     <r>
@@ -788,16 +1252,86 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> to its engineering practices whenever needed. 
+      <t xml:space="preserve"> to its engineering practices whenever needed.
 </t>
     </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>User story</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : se rédige comme suit : en tant que, je veux, afin de. 
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Plan of work for next 24h, inspecting work since the last, forecasting upcoming sprint work.
+Developers only, 15 minutes peu importe la taille de l'équipe, debout ou pas, tous les jours, le matin.
+BEFORE : 3 questions &gt; hier, aujourd'hui, blocages. NOW : </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">questions ou discussion, tout est possible.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Le scrum master ne la "conduit" pas.
+3 questions du scrum master : je vois les obstacles qui empêchent d'aller au but, j'ai vu hier ce qui peut aider les developers, je peux les aider aujourd'hui à atteindre ce but. 
+--NO CANCELLATION ALLOWED--</t>
+    </r>
+  </si>
+  <si>
+    <t>KANBAN</t>
+  </si>
+  <si>
+    <t>Sur le tableau avec les colonnes, limiter le "en cours" (Work In Progress).</t>
+  </si>
+  <si>
+    <t>Definition of Ready
+DOR</t>
+  </si>
+  <si>
+    <t>La user story est claire, précise et comprise. Pour la scrum team, le PO peut y assister. Se fait n'importe quand.</t>
+  </si>
+  <si>
+    <t>Definition of DONE
+DOD</t>
   </si>
   <si>
     <r>
       <t xml:space="preserve">sprint backlog, product backlog, defintion of done, increment (à voir).   
 Inspect frequently, but it should not get in the way of the work.   Sprint goal provides guidance.
 PILARS : TIA &gt; transparency (responsable scrum master), adaptation, inspection. Le PO monitore.
-Increment (livrable respectant le DOD*) : somme de tous les product backlog items and the value, </t>
+Increment (livrable respectant le DOD) : somme de tous les product backlog items and the value, </t>
     </r>
     <r>
       <rPr>
@@ -818,43 +1352,15 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>, géré par le PO, valuable when it reduces operational costs and increases customer satisfasfaction, includes regression testing. 
+      <t xml:space="preserve">, géré par le PO, valuable when it reduces operational costs and increases customer satisfasfaction, includes regression testing. 
 Si retard dû à un élément manquant, être sûr d'avoir des tâches à faire pour le prochain sprint en attendant.
-*DOD : definition of done.</t>
-    </r>
-  </si>
-  <si>
-    <t>ils mélangent les versions (ancienne/nouvelle) dans les questions de la certif. Si dans la question, il y a "dev team" : ancienne, 
-si "developers" : nouvelle.</t>
-  </si>
-  <si>
-    <t>Definition of DONE</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">C'est un servant leader sans pouvoir, helping developers to create value, removing impediments, coaching the developers.
 </t>
     </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Is responsible for conducting the Daily Scrum</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">. NOW : Il est </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">8h max pour 1 mois et si moins alors "less",  responsable: scrum team, pas la place des stakeholders mais ils peuvent y assister.
+Participants : la scrum team (scrum master, product owner, developers). Others possible to provide </t>
     </r>
     <r>
       <rPr>
@@ -865,591 +1371,21 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>responsable</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> de la réussite de la scrum team.
-Leading &amp; coaching org, working with other scrum masters, planning scrum implementations.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Facilitating</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> and teaching scrum events, </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>techniques for product backlog management</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, empirical env.
-Si le PO a des soucis avec les user stories, il peut les rédiger.</t>
-    </r>
-  </si>
-  <si>
-    <t>Sprint Review
-(événement scrum)</t>
-  </si>
-  <si>
-    <t>Sprint rétrospective
-(événement scrum)</t>
-  </si>
-  <si>
-    <t>Sprint planning
-(événement scrum)</t>
-  </si>
-  <si>
-    <t>Daily Scrum
-(événement scrum)</t>
-  </si>
-  <si>
-    <t>1 mois : 20 jours de travail.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Cancellation</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> : PO only (OR </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>if sprint goal obsolete ( ou inatteignable)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">). Le sprint zero n'existe pas.
-Longueur maximale : 1 mois sinon, pas de norme selon de scrum guide MAIS on établit sa </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>longueur</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> en fonction : de la possibilité d'être en réunion avec les stakeholders et des "done" pouvant être faits + fréquemment.
-La qualité ne doit pas baisser, l'objectif ne doit pas être mis en danger, scope may be clarified and re-negociated.
-Le sprint est le SEUL moment dans lequel </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>on n'inspecte pas et on n'adapte pas</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">.
-Durant le sprint &gt; choix des besoins livrables le mois, spec f, dev, test, livraison.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">At the end </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>of the sprint : the delivery is working, functional, DONE.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Plan of work for next 24h, inspecting work since the last, forecasting upcoming sprint work.
-Dev team, 15 minutes peu importe la taille de l'équipe, debout ou pas, tous les jours, le matin ou l'après-midi.
-BEFORE : 3 questions &gt; hier, aujourd'hui, blocages. NOW : </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">questions ou discussion, tout est possible.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Le scrum master ne la "conduit" pas.
-3 questions du scrum master : je vois les obstacles qui empêchent d'aller au but, j'ai vu hier ce qui peut aider les developers, je peux les aider aujourd'hui à atteindre ce but. --NO CANCELLATION ALLOWED--.</t>
-    </r>
-  </si>
-  <si>
-    <t>Backlog Refinement 
-ou Grooming
-(non événement)</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Le PO, developers. BEFORE : "consume not more than 10% of the capacity of the developers"    NOW : à l'appréciation.
-Not for the current sprint in progress, on prépare le sprint suivant à la mi-sprint, durée à la convenance.
-Ongoing process, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>act of adding detail</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Responsable : PO uniquement.
-Les developers peuvent faire des changements </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>avec l'accord du PO (attention au sens de la question)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Les developers sont responsable des </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">estimations.      </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Any technique should be used for </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>representing</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> product backlog items. Ce qui n'est pas fini n'est pas reporté au prochain sprint, c'est mis dans le product backlog.
-developers </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>should</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> use the same product backlog.    </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Ready</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> : well refined, at the top, can be done in 1 sprint.
-&gt; dynamic, never complete, existe tant que le produit existe.
-C'est </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>la seule source</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> pour tout changement du produit.     </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Optionnel</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> : tests prouvant le "done" et les dépendances.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Management : </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">PO responsable.
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">3 heures max, cérémonie scrum en fermeture du sprint qui se réalise juste après la sprint Review. C'est pour la scrum team, donc le PO y participe et peut adapter le "done". 
-( pour les processus) Sert à </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>améliorer</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> pour les prochains sprints, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>identifier</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> ce qui a été bien et qui a du potentiel d'amélioration, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>analyser</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> ce qui s'est passé &gt;&gt; &gt;&gt;&gt; people, relationships, process, and tool.
-if </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>improvement</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> possible, include at least 1 high priority process for the next.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Pour toute question où il y a la notion d'obligation, la réponse sera </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>FALSE</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">8h max (4h/2semaines, 8h/1mois), responsable: scrum team, pas la place des stakeholders mais ils peuvent y assister.
-Participants : la scrum team (scrum master, product owner, developers). Others possible to provide </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>technical advice</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">.
+      <t xml:space="preserve">technical advice </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">TOUT LE MONDE PEUT Y ASSISTER.
 Comment le travail sera fait pour le prochain increment ? (work needed to deliver)
 Qu'est-ce qui sera livré? (delivered in the Increment resulting).
 Le BA rédige les user stories.
-les questions sur le choix des user stories : why, what, how. 
+NEW : Les questions sur le choix des user stories : why (sprint goal), what (product backlog items), how (tasks). 
 </t>
     </r>
     <r>
@@ -1493,7 +1429,102 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>. Les developers se défendent avec la vélocité.</t>
+      <t>. Les developers se défendent avec la vélocité (Business Value pour le client, Story Points pour la scrum team).</t>
+    </r>
+  </si>
+  <si>
+    <t>4 heures max pour 1 mois et si moins alors "less", but : présenter le produit (travail réalisé) durant le sprint en cours OU "a revisited product backlog", inspecter le résultat. 
+C'est pour les stakeholders, scrum master, developers, PO, TOUT LE MONDE PEUT Y ASSISTER.   It's not JUST a demo et possible de ne rien livrer.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">3 heures max, cérémonie scrum en fermeture du sprint qui se réalise juste après la sprint Review. C'est pour la scrum team, donc le PO y participe et peut adapter le "done". 
+( pour les processus) Sert à </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>améliorer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> pour les prochains sprints, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>identifier</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ce qui a été bien et qui a du potentiel d'amélioration (continue), </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>analyser</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ce qui s'est passé &gt;&gt; &gt;&gt;&gt; people, relationships, process, and tool.
+if </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>improvement</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> possible, include at least 1 high priority process for the next.</t>
     </r>
   </si>
 </sst>
@@ -1574,14 +1605,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="14"/>
       <color theme="1"/>
@@ -1604,6 +1627,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1611,12 +1642,6 @@
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -1636,8 +1661,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -1645,11 +1676,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1660,25 +1706,43 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1966,10 +2030,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C38"/>
+  <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="18" x14ac:dyDescent="0.3"/>
@@ -1981,205 +2045,315 @@
     <col min="5" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="C1" s="6" t="s">
+    <row r="1" spans="1:3" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="161.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="8"/>
+    </row>
+    <row r="4" spans="1:3" ht="80.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="12.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="8"/>
+    </row>
+    <row r="6" spans="1:3" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="12.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="8"/>
+    </row>
+    <row r="8" spans="1:3" ht="159" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="8"/>
+    </row>
+    <row r="10" spans="1:3" ht="174" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="14"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="8"/>
+    </row>
+    <row r="12" spans="1:3" ht="165.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="8"/>
+    </row>
+    <row r="13" spans="1:3" ht="12.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="4"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="8"/>
+    </row>
+    <row r="14" spans="1:3" ht="79.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="14"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="8"/>
+    </row>
+    <row r="16" spans="1:3" ht="84.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="8"/>
+    </row>
+    <row r="17" spans="1:3" ht="12.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="4"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="8"/>
+    </row>
+    <row r="18" spans="1:3" ht="102" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="8"/>
+    </row>
+    <row r="19" spans="1:3" ht="12.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="4"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="8"/>
+    </row>
+    <row r="20" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="8"/>
+    </row>
+    <row r="21" spans="1:3" ht="12.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="4"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="8"/>
+    </row>
+    <row r="22" spans="1:3" ht="190.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" s="8"/>
+    </row>
+    <row r="23" spans="1:3" ht="12.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="4"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="8"/>
+    </row>
+    <row r="24" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24" s="8"/>
+    </row>
+    <row r="25" spans="1:3" ht="12.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="4"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="8"/>
+    </row>
+    <row r="26" spans="1:3" ht="147" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" s="8"/>
+    </row>
+    <row r="27" spans="1:3" ht="12.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="4"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="8"/>
+    </row>
+    <row r="28" spans="1:3" ht="135" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" s="8"/>
+    </row>
+    <row r="29" spans="1:3" ht="12.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="4"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="8"/>
+    </row>
+    <row r="30" spans="1:3" ht="160.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C30" s="8"/>
+    </row>
+    <row r="31" spans="1:3" ht="12.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="4"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="8"/>
+    </row>
+    <row r="32" spans="1:3" ht="184.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" s="5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="161.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="4"/>
-    </row>
-    <row r="4" spans="1:3" ht="60.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="12.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:3" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+      <c r="C32" s="8"/>
+    </row>
+    <row r="33" spans="1:3" ht="12.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="4"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="8"/>
+    </row>
+    <row r="34" spans="1:3" ht="161.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="4"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="8"/>
+    </row>
+    <row r="36" spans="1:3" ht="144" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C36" s="8"/>
+    </row>
+    <row r="37" spans="1:3" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="4"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="8"/>
+    </row>
+    <row r="38" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A38" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B38" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="1" t="s">
+      <c r="C38" s="8"/>
+    </row>
+    <row r="39" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="4"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="8"/>
+    </row>
+    <row r="40" spans="1:3" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C40" s="8"/>
+    </row>
+    <row r="41" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="4"/>
+      <c r="B41" s="5"/>
+      <c r="C41" s="8"/>
+    </row>
+    <row r="42" spans="1:3" ht="91.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="12.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:3" ht="79.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="12.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:3" ht="159" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="12.6" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:3" ht="174" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="9"/>
-    </row>
-    <row r="14" spans="1:3" ht="165.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" s="2" t="s">
+      <c r="B42" s="5" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" ht="12.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:3" ht="84.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="12.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="18" spans="1:3" ht="102" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="12.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="20" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="12.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="1:3" ht="190.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="12.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="24" spans="1:3" ht="147" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="12.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="26" spans="1:3" ht="135" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="12.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="28" spans="1:3" ht="160.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="12.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="1:3" ht="184.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="12.45" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="32" spans="1:3" ht="161.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="12.6" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="34" spans="1:2" ht="144" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="12.6" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="36" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A36" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="38" spans="1:2" ht="91.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>27</v>
-      </c>
+      <c r="C42" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
correction 4 avec cours de M
</commit_message>
<xml_diff>
--- a/prepa_certif_updated_scrum_questions_faites.xlsx
+++ b/prepa_certif_updated_scrum_questions_faites.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\formation_BA\Nouveau dossier\prepa_certif\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F830431C-A94C-4590-83BF-3118858C2441}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5469E79F-ED19-4DB2-9985-629822973B72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,9 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
   <si>
-    <t>Burndown chart</t>
-  </si>
-  <si>
     <t>Product backlog</t>
   </si>
   <si>
@@ -77,106 +74,6 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> est pour le PO.</t>
-    </r>
-  </si>
-  <si>
-    <t>Scrum master, product owner, developers.  
-Différentes équipes scrum d'un même produit peuvent NE PAS avoir des sprints de longueur différente (does not require) et ne pas avoir de sprint "alignés".
-Elle fait le SPRINT PLANNING, responsible for crafting the sprint goal during it. Elle doit être autosuffisante.
-Qualités importantes : flexibility, creativity, productivity.
-Should have all competencies, should choose how best to accomplish their work.
-If a 2nd scrum team is added, productivity is likely to decrease.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Developers (responsable du suivi du travail restant), la définition de "done" </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>créée par les developers</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> peut possiblement </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>s'adapter</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> à chaque RETRO </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>par la scrum team</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, n'aide pas à calculer la vélocité.
-DONE est l'objectif, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>pas la réduction de la dette technique par un sprint spécial (hardening)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.
-Doit respecter : conventions &amp; standards, same definition for other teams working on the same product.
-ensures artifact transparency, is used to acces, guides the developers.</t>
     </r>
   </si>
   <si>
@@ -403,13 +300,6 @@
     </r>
   </si>
   <si>
-    <t>How much work remains till the end of the sprint, shows the evolution of remaining effort against time.
-Responsable : developers.</t>
-  </si>
-  <si>
-    <t>Le mot scrum est apparu en 1995, l'agilité en 2001, le scrum guide en 2010.</t>
-  </si>
-  <si>
     <t>ils mélangent les versions (ancienne/nouvelle) dans les questions de la certif. Si dans la question, il y a "dev team" : ancienne, 
 si "developers" : nouvelle.</t>
   </si>
@@ -1330,145 +1220,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">user-story, velocity, definition of ready &gt;&gt; tous ces termes n'existent pas dans le guide scrum.
-La vélocité est une mesure de la </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>maturité</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> de l'équipe, pas un indice de réussite.
-Composition des équipes de dev en fonction de la </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"self-organization"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">.
-Developers : </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Adjustments</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> to its engineering practices whenever needed.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>User story</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> : se rédige comme suit : en tant que, je veux, afin de. 
-Méthode </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Moscow</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> pour </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>prioriser</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> selon les points accordés aux Should et Could.
-Planning Poker : story points estimés avec la business value et la complexité de dév.
-(points des dev : prendre le max et le min, si trop grand écart, réévaluer sinon la moyenne).
-</t>
-    </r>
-  </si>
-  <si>
     <t>Increment</t>
   </si>
   <si>
@@ -1597,6 +1348,282 @@
   </si>
   <si>
     <t>rolling wave, sans fin.</t>
+  </si>
+  <si>
+    <t>Burndup/Burndown chart, KPI</t>
+  </si>
+  <si>
+    <t>How much work remains till the end of the sprint, shows the evolution of remaining effort against time. 
+NEW : KPI &gt; cumulative flow diagram : reduire la colonne "en cours".
+NEW : KPI &gt; vélocité :  des story points (mesure sur 5 sprints), pour savoir nbre pts/sprint.
+UP : Outil non précis et ne prévoit pas.
+DOWN : analyse de tendance et prévision.
+Responsable : developers.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Developers (responsable du suivi du travail restant), la définition de "done" </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>créée par les developers</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> peut possiblement </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>s'adapter</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> à chaque RETRO </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>par la scrum team</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, n'aide pas à calculer la vélocité.
+DONE est l'objectif, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>pas la réduction de la dette technique par un sprint spécial (hardening)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.
+Doit respecter : conventions &amp; standards, same definition for other teams working on the same product, pas de travail supplémentaire à faire.
+ensures artifact transparency, is used to acces, guides the developers.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">user-story, velocity, definition of ready &gt;&gt; tous ces termes n'existent pas dans le guide scrum.
+La vélocité est une mesure de la </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>maturité</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> de l'équipe, pas un indice de réussite.
+Composition des équipes de dev en fonction de la </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"self-organization"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">.
+Developers : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Adjustments</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> to its engineering practices whenever needed.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>User story</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : se rédige comme suit : en tant que, je veux, afin de. 
+Méthode </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Moscow</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> pour </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>prioriser</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> selon les points accordés aux Should et Could.
+Planning Poker : story points estimés avec la business value et la complexité de dév.
+(points des dev : prendre le max et le min, si trop grand écart, réévaluer sinon la moyenne).
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Dette technique : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">non respect de la conception voulue ou non induisant des coûts supplémentaires vus comme des interêts.
+</t>
+    </r>
+  </si>
+  <si>
+    <t>Scrum master, product owner, developers.  
+Différentes équipes scrum d'un même produit peuvent NE PAS avoir des sprints de longueur différente (does not require) et ne pas avoir de sprint "alignés".
+Elle fait le SPRINT PLANNING, responsible for crafting the sprint goal during it. Elle doit être autosuffisante.
+Qualités importantes : flexibility, creativity, productivity.
+Should have all competencies, should choose how best to accomplish their work.
+If a 2nd scrum team is added, productivity is likely to decrease.
+BEFORE : self-organizing, NOW : self-managing.</t>
+  </si>
+  <si>
+    <t>Le mot scrum est apparu en 1995, l'agilité en 2001, le 1er scrum guide en 2011, le 2ème en 2020.</t>
   </si>
 </sst>
 </file>
@@ -2124,7 +2151,7 @@
   <dimension ref="A1:C44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2140,18 +2167,18 @@
       <c r="A1" s="12"/>
       <c r="B1" s="3"/>
       <c r="C1" s="10" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="161.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -2159,15 +2186,15 @@
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
     </row>
-    <row r="4" spans="1:3" ht="80.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="12.45" customHeight="1" x14ac:dyDescent="0.3">
@@ -2177,13 +2204,13 @@
     </row>
     <row r="6" spans="1:3" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="12.45" customHeight="1" x14ac:dyDescent="0.3">
@@ -2193,13 +2220,13 @@
     </row>
     <row r="8" spans="1:3" ht="159" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2209,13 +2236,13 @@
     </row>
     <row r="10" spans="1:3" ht="174" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2225,10 +2252,10 @@
     </row>
     <row r="12" spans="1:3" ht="165.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="14" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C12" s="5"/>
     </row>
@@ -2239,13 +2266,13 @@
     </row>
     <row r="14" spans="1:3" ht="79.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="16" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>19</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2255,10 +2282,10 @@
     </row>
     <row r="16" spans="1:3" ht="84.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="14" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C16" s="5"/>
     </row>
@@ -2269,10 +2296,10 @@
     </row>
     <row r="18" spans="1:3" ht="102" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="14" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C18" s="5"/>
     </row>
@@ -2283,10 +2310,10 @@
     </row>
     <row r="20" spans="1:3" ht="96" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="12" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C20" s="5"/>
     </row>
@@ -2297,10 +2324,10 @@
     </row>
     <row r="22" spans="1:3" ht="190.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="12" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C22" s="5"/>
     </row>
@@ -2311,10 +2338,10 @@
     </row>
     <row r="24" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="12" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C24" s="5"/>
     </row>
@@ -2325,10 +2352,10 @@
     </row>
     <row r="26" spans="1:3" ht="147" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="12" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>10</v>
+        <v>48</v>
       </c>
       <c r="C26" s="5"/>
     </row>
@@ -2339,10 +2366,10 @@
     </row>
     <row r="28" spans="1:3" ht="87.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="12" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C28" s="5"/>
     </row>
@@ -2353,10 +2380,10 @@
     </row>
     <row r="30" spans="1:3" ht="135" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="12" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>9</v>
+        <v>50</v>
       </c>
       <c r="C30" s="5"/>
     </row>
@@ -2367,10 +2394,10 @@
     </row>
     <row r="32" spans="1:3" ht="160.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="12" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C32" s="5"/>
     </row>
@@ -2381,13 +2408,13 @@
     </row>
     <row r="34" spans="1:3" ht="184.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="12.45" customHeight="1" x14ac:dyDescent="0.3">
@@ -2397,13 +2424,13 @@
     </row>
     <row r="36" spans="1:3" ht="161.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2413,10 +2440,10 @@
     </row>
     <row r="38" spans="1:3" ht="144" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C38" s="5"/>
     </row>
@@ -2427,10 +2454,10 @@
     </row>
     <row r="40" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A40" s="12" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C40" s="5"/>
     </row>
@@ -2441,10 +2468,10 @@
     </row>
     <row r="42" spans="1:3" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="12" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C42" s="5"/>
     </row>
@@ -2453,12 +2480,12 @@
       <c r="B43" s="3"/>
       <c r="C43" s="5"/>
     </row>
-    <row r="44" spans="1:3" ht="135.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" ht="156.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="12" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C44" s="5"/>
     </row>

</xml_diff>

<commit_message>
correction 5 avec cours de M
</commit_message>
<xml_diff>
--- a/prepa_certif_updated_scrum_questions_faites.xlsx
+++ b/prepa_certif_updated_scrum_questions_faites.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\formation_BA\Nouveau dossier\prepa_certif\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5469E79F-ED19-4DB2-9985-629822973B72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC6A78B7-AD07-4AF7-A098-43F3320626F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -184,122 +184,6 @@
     <t>proxy PO : son adjoint</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Sa responsabilité : la product backlog, pas le produit ni du delivery.
-Interêts : le produit, ordering items, optimizing value, keep visible &amp; transparent the work on next., les stakholder ( le PO prend le feedback de ces derniers pour évaluer la VALEUR).
-monitoring progress toward high-level </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>goals.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">   He is the chief product </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>visionary</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>KVA</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> : current value, ability to innovate, time-to-market (expert).
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Pas le problème du PO :</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> coach the developers, remove impediments to the developers.
-Iterating vision every sprint, planning features, articulating the product vision (early and often).
-Releases ? C'est le PO </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>qui décide la mise en prod</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>... the risk for the value, absorption by the customer, the costs and benefits, the constraints by the new release.Il peut déléguer l'écriture des user-stories aux developers mais il en est responsable.</t>
-    </r>
-  </si>
-  <si>
     <t>ils mélangent les versions (ancienne/nouvelle) dans les questions de la certif. Si dans la question, il y a "dev team" : ancienne, 
 si "developers" : nouvelle.</t>
   </si>
@@ -589,37 +473,6 @@
   <si>
     <t>Sprint 
 (événement scrum)</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Plan of work for next 24h, inspecting work since the last, forecasting upcoming sprint work.
-Developers only, 15 minutes peu importe la taille de l'équipe, debout ou pas, tous les jours, le matin.
-BEFORE : 3 questions &gt; hier, aujourd'hui, blocages. NOW : </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">questions ou discussion, tout est possible.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Le scrum master ne la "conduit" pas.
-3 questions du scrum master : je vois les obstacles qui empêchent d'aller au but, j'ai vu hier ce qui peut aider les developers, je peux les aider aujourd'hui à atteindre ce but. 
---NO CANCELLATION ALLOWED--</t>
-    </r>
   </si>
   <si>
     <t>KANBAN</t>
@@ -1450,167 +1303,6 @@
       <t>.
 Doit respecter : conventions &amp; standards, same definition for other teams working on the same product, pas de travail supplémentaire à faire.
 ensures artifact transparency, is used to acces, guides the developers.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">user-story, velocity, definition of ready &gt;&gt; tous ces termes n'existent pas dans le guide scrum.
-La vélocité est une mesure de la </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>maturité</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> de l'équipe, pas un indice de réussite.
-Composition des équipes de dev en fonction de la </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"self-organization"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">.
-Developers : </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Adjustments</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> to its engineering practices whenever needed.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>User story</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> : se rédige comme suit : en tant que, je veux, afin de. 
-Méthode </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Moscow</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> pour </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>prioriser</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> selon les points accordés aux Should et Could.
-Planning Poker : story points estimés avec la business value et la complexité de dév.
-(points des dev : prendre le max et le min, si trop grand écart, réévaluer sinon la moyenne).
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Dette technique : </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">non respect de la conception voulue ou non induisant des coûts supplémentaires vus comme des interêts.
-</t>
     </r>
   </si>
   <si>
@@ -1624,6 +1316,315 @@
   </si>
   <si>
     <t>Le mot scrum est apparu en 1995, l'agilité en 2001, le 1er scrum guide en 2011, le 2ème en 2020.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">burndown chart &gt;&gt; tous ces termes n'existent pas dans le guide scrum.
+La vélocité est une mesure de la </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>maturité</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> de l'équipe, pas un indice de réussite.
+Composition des équipes de dev en fonction de la </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"self-organization"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">.
+Developers : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Adjustments</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> to its engineering practices whenever needed.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>User story</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : se rédige comme suit : en tant que, je veux, afin de. 
+Méthode </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Moscow</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> pour </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>prioriser</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> selon les points accordés aux Should et Could.
+Planning Poker : story points estimés avec la business value et la complexité de dév.
+(points des dev : prendre le max et le min, si trop grand écart, réévaluer sinon la moyenne).
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Dette technique : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">non respect de la conception voulue ou non induisant des coûts supplémentaires vus comme des interêts.
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Plan of work for next 24h, inspecting work since the last, forecasting upcoming sprint work.
+Developers only, 15 minutes peu importe la taille de l'équipe, debout ou pas, tous les jours, le matin, toujours au même endroit.
+BEFORE : 3 questions &gt; hier, aujourd'hui, blocages. NOW : </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">questions ou discussion, tout est possible.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Le scrum master ne la "conduit" pas.
+3 questions du scrum master : je vois les obstacles qui empêchent d'aller au but, j'ai vu hier ce qui peut aider les developers, je peux les aider aujourd'hui à atteindre ce but. 
+--NO CANCELLATION ALLOWED--</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Sa responsabilité : la product backlog, pas le produit ni du delivery.
+Interêts : le produit, ordering items, optimizing value, keep visible &amp; transparent the work on next., les stakholder ( le PO prend le feedback de ces derniers pour évaluer la VALEUR).
+monitoring progress toward high-level </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>goals.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">   He is the chief product </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>visionary</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>KVA</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : current value, ability to innovate, time-to-market (expert).
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Pas le problème du PO :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> coach the developers, remove impediments to the developers.
+Iterating vision every sprint, planning features, articulating the product vision (early and often).
+Releases ? C'est le PO </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>qui décide la mise en prod</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>... the risk for the value, absorption by the customer, the costs and benefits, the constraints by the new release.Il peut déléguer l'écriture des user-stories aux developers mais il en est responsable.
+Il n'assigne AUCUNE tâche aux developers.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2150,8 +2151,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2175,10 +2176,10 @@
         <v>8</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -2188,13 +2189,13 @@
     </row>
     <row r="4" spans="1:3" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="12.45" customHeight="1" x14ac:dyDescent="0.3">
@@ -2207,7 +2208,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>9</v>
@@ -2220,13 +2221,13 @@
     </row>
     <row r="8" spans="1:3" ht="159" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2236,13 +2237,13 @@
     </row>
     <row r="10" spans="1:3" ht="174" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2252,10 +2253,10 @@
     </row>
     <row r="12" spans="1:3" ht="165.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="C12" s="5"/>
     </row>
@@ -2266,13 +2267,13 @@
     </row>
     <row r="14" spans="1:3" ht="79.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="7" t="s">
-        <v>24</v>
-      </c>
       <c r="C14" s="5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2282,10 +2283,10 @@
     </row>
     <row r="16" spans="1:3" ht="84.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C16" s="5"/>
     </row>
@@ -2296,10 +2297,10 @@
     </row>
     <row r="18" spans="1:3" ht="102" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C18" s="5"/>
     </row>
@@ -2313,7 +2314,7 @@
         <v>2</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C20" s="5"/>
     </row>
@@ -2327,7 +2328,7 @@
         <v>0</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C22" s="5"/>
     </row>
@@ -2338,10 +2339,10 @@
     </row>
     <row r="24" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C24" s="5"/>
     </row>
@@ -2352,10 +2353,10 @@
     </row>
     <row r="26" spans="1:3" ht="147" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C26" s="5"/>
     </row>
@@ -2366,10 +2367,10 @@
     </row>
     <row r="28" spans="1:3" ht="87.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C28" s="5"/>
     </row>
@@ -2380,10 +2381,10 @@
     </row>
     <row r="30" spans="1:3" ht="135" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="12" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C30" s="5"/>
     </row>
@@ -2397,7 +2398,7 @@
         <v>1</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C32" s="5"/>
     </row>
@@ -2414,7 +2415,7 @@
         <v>11</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="12.45" customHeight="1" x14ac:dyDescent="0.3">
@@ -2422,12 +2423,12 @@
       <c r="B35" s="3"/>
       <c r="C35" s="5"/>
     </row>
-    <row r="36" spans="1:3" ht="161.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" ht="182.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>13</v>
@@ -2443,7 +2444,7 @@
         <v>5</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C38" s="5"/>
     </row>
@@ -2468,10 +2469,10 @@
     </row>
     <row r="42" spans="1:3" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C42" s="5"/>
     </row>

</xml_diff>